<commit_message>
phong dang ki roi
phong dang ki roi
</commit_message>
<xml_diff>
--- a/danh sach.xlsx
+++ b/danh sach.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>STT</t>
   </si>
@@ -25,6 +25,12 @@
   </si>
   <si>
     <t>ten</t>
+  </si>
+  <si>
+    <t>thanh</t>
+  </si>
+  <si>
+    <t>phong</t>
   </si>
 </sst>
 </file>
@@ -382,7 +388,7 @@
   <dimension ref="C6:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -402,8 +408,12 @@
       <c r="C7" s="1">
         <v>1</v>
       </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
+      <c r="D7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="8" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C8" s="1">

</xml_diff>